<commit_message>
Added escalations for cases
</commit_message>
<xml_diff>
--- a/Tools/Links.xlsx
+++ b/Tools/Links.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\My Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\My Documents\Amazon-Links\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D720E68E-A35A-430E-A802-055BFF533A52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47C0780-EC15-4FEC-A564-0F017F8B3A46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Links" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
   <si>
     <t>BRS1 LINKS</t>
   </si>
@@ -113,27 +113,6 @@
     <t>Case Tracker</t>
   </si>
   <si>
-    <t>CC-RM-GB-H1-2D-LR</t>
-  </si>
-  <si>
-    <t>CC-RM-GB-H1-3D-LR</t>
-  </si>
-  <si>
-    <t>CC-RM-GB-H1-HV-F-VCRI</t>
-  </si>
-  <si>
-    <t>LMC</t>
-  </si>
-  <si>
-    <t>CC-RM-GB-H1-ND-F-VCRI</t>
-  </si>
-  <si>
-    <t>CC-RM-GB-H1-ND-LR</t>
-  </si>
-  <si>
-    <t>BRISTOL H1 17:00</t>
-  </si>
-  <si>
     <t>TSO Screen</t>
   </si>
   <si>
@@ -168,13 +147,109 @@
   </si>
   <si>
     <t>eu-roc-ob-cancel-truck@amazon.com</t>
+  </si>
+  <si>
+    <t>Escalation level</t>
+  </si>
+  <si>
+    <t>Escalation Pre-Requisites</t>
+  </si>
+  <si>
+    <t>E-Mail</t>
+  </si>
+  <si>
+    <t>Level 1</t>
+  </si>
+  <si>
+    <t>1 hour from case creation with no response. Please do not include ROC escalation e-mail when opening a case. The escalations will only be addressed if there is an existing case.</t>
+  </si>
+  <si>
+    <t>Contact DM Transportation Leads</t>
+  </si>
+  <si>
+    <t>eu-roc-dm-escalation-level1@amazon.com</t>
+  </si>
+  <si>
+    <t>Level 2</t>
+  </si>
+  <si>
+    <r>
+      <t>No response from 1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>st</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Level escalation after 2 hours or impact in the next 30 min which could have a Safety/Security, CX impact, or logistic issue</t>
+    </r>
+  </si>
+  <si>
+    <t>Contact DM Transportation Managers</t>
+  </si>
+  <si>
+    <t>eu-roc-dm-escalation-level2@amazon.com</t>
+  </si>
+  <si>
+    <t>Level 3</t>
+  </si>
+  <si>
+    <r>
+      <t>No response from 2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Level escalation after 3 hours or a critical issue (Sev1) that needs immediate attention</t>
+    </r>
+  </si>
+  <si>
+    <t>Contact DM Transportation Snr Managers</t>
+  </si>
+  <si>
+    <t>eu-roc-dm-escalation-level3@amazon.com</t>
+  </si>
+  <si>
+    <t>Level 4</t>
+  </si>
+  <si>
+    <t>Snr Manager EU ROC DM - Ana Gil Ferrer – frrran@amazon.es</t>
+  </si>
+  <si>
+    <t>eu-roc-dm-snrmanagers@amazon.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,8 +284,34 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,8 +330,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7CAAC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -378,6 +497,93 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF666666"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF666666"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF999999"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF999999"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF999999"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF666666"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF999999"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -386,7 +592,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -395,9 +601,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -417,6 +620,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -426,9 +635,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -459,11 +665,41 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -786,15 +1022,15 @@
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
@@ -830,44 +1066,44 @@
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D10" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
+      <c r="D10" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D11" s="31" t="s">
@@ -892,147 +1128,147 @@
       <c r="J12" s="30"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="21"/>
     </row>
     <row r="17" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
     </row>
     <row r="18" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D18" s="21" t="s">
+      <c r="D18" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D21" s="21" t="s">
+      <c r="D21" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D22" s="21" t="s">
+      <c r="D22" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
     </row>
     <row r="23" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D23" s="21" t="s">
+      <c r="D23" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
     </row>
     <row r="25" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D25" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="20"/>
+      <c r="D25" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="21"/>
     </row>
     <row r="27" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D27" s="2"/>
@@ -1045,15 +1281,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="D22:J22"/>
-    <mergeCell ref="D17:J17"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="D20:J20"/>
-    <mergeCell ref="D16:J16"/>
-    <mergeCell ref="D21:J21"/>
-    <mergeCell ref="D18:J18"/>
-    <mergeCell ref="D19:J19"/>
-    <mergeCell ref="D10:J10"/>
     <mergeCell ref="D25:J25"/>
     <mergeCell ref="D24:J24"/>
     <mergeCell ref="D2:J2"/>
@@ -1070,6 +1297,15 @@
     <mergeCell ref="D13:J13"/>
     <mergeCell ref="D14:J14"/>
     <mergeCell ref="D11:J11"/>
+    <mergeCell ref="D22:J22"/>
+    <mergeCell ref="D17:J17"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="D20:J20"/>
+    <mergeCell ref="D16:J16"/>
+    <mergeCell ref="D21:J21"/>
+    <mergeCell ref="D18:J18"/>
+    <mergeCell ref="D19:J19"/>
+    <mergeCell ref="D10:J10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4:J4" r:id="rId1" display="Old Links Page" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -1101,8 +1337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C875AD2B-934E-44BC-9193-03D830E2EB51}">
   <dimension ref="B2:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,10 +1351,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="12"/>
+      <c r="B2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="11"/>
       <c r="D2" s="4" t="s">
         <v>19</v>
       </c>
@@ -1128,15 +1364,15 @@
       <c r="F2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="17" t="s">
-        <v>41</v>
+      <c r="G2" s="16" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="11"/>
+      <c r="B3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="10"/>
       <c r="E3" s="4" t="s">
         <v>20</v>
       </c>
@@ -1145,32 +1381,32 @@
       </c>
     </row>
     <row r="4" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="11"/>
+      <c r="B4" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="10"/>
       <c r="E4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="11"/>
+      <c r="B5" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="10"/>
       <c r="E5" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="11"/>
+      <c r="B6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="10"/>
       <c r="F6" s="6" t="s">
         <v>25</v>
       </c>
@@ -1178,44 +1414,44 @@
     <row r="7" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="12"/>
+      <c r="B9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="11"/>
     </row>
     <row r="10" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="11"/>
+      <c r="B11" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="10"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="11"/>
+      <c r="B12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="10"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="11"/>
+      <c r="B13" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="10"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L16" s="8"/>
+      <c r="L16" s="7"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1225,57 +1461,111 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38BDF580-501A-4050-B541-44176D985EDE}">
-  <dimension ref="B3:C8"/>
+  <dimension ref="B1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="33"/>
-      <c r="C4" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="33"/>
-      <c r="C5" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="33"/>
-      <c r="C8" s="7" t="s">
-        <v>33</v>
+    <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="75.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="38"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="B5" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="38"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="B7" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="38"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B3:B5"/>
+  <mergeCells count="6">
     <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" display="https://w.amazon.com/bin/view/ROC_EU/FC_SC_Handbook/Issuein48hrs/Casecreation/" xr:uid="{F5AC8034-0E2A-4BFB-B57F-A4B01DE6419E}"/>
+    <hyperlink ref="D4" r:id="rId2" display="mailto:eu-roc-dm-escalation-level1@amazon.com" xr:uid="{79C1C778-8FAC-4041-BEDF-A4541EA03EEE}"/>
+    <hyperlink ref="D6" r:id="rId3" display="mailto:eu-roc-dm-escalation-level2@amazon.com" xr:uid="{6480480A-CFC8-46E1-B485-CB7C31E82EC0}"/>
+    <hyperlink ref="D8" r:id="rId4" display="mailto:eu-roc-dm-escalation-level3@amazon.com" xr:uid="{47650181-EA4C-4E3C-B458-8C87E66EF06E}"/>
+    <hyperlink ref="C9" r:id="rId5" display="mailto:frrran@amazon.es" xr:uid="{EBEFF933-F2A4-4B8D-A42B-7726878CF558}"/>
+    <hyperlink ref="D9" r:id="rId6" display="mailto:eu-roc-dm-snrmanagers@amazon.com" xr:uid="{16BEB41A-4713-4AC7-9821-CB57E67D0924}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>